<commit_message>
Finish ethics checklist (#14)
* Update ethics checklist

* Use the checklist change to add detail
</commit_message>
<xml_diff>
--- a/report/ethics/ethics-checklist-ug.xlsx
+++ b/report/ethics/ethics-checklist-ug.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\matbon\thesis\report\ethics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08435E49-F9C2-4CC5-9815-D527F62F99A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181E7C81-0489-4751-8E7C-452A6BF1C016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>Section 1: HUMANS</t>
   </si>
@@ -580,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +652,9 @@
     <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>